<commit_message>
Updated parts tracking sheet
</commit_message>
<xml_diff>
--- a/Dokumentace/Dokumentační podklady/Objednané součástky/Sledování součástek.xlsx
+++ b/Dokumentace/Dokumentační podklady/Objednané součástky/Sledování součástek.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Odkaz</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Klon Arduino Due</t>
+  </si>
+  <si>
+    <t>Předpokládané přijetí</t>
   </si>
 </sst>
 </file>
@@ -68,9 +71,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;Kč&quot;_-;\-* #,##0.00\ &quot;Kč&quot;_-;_-* &quot;-&quot;??\ &quot;Kč&quot;_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +94,15 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -120,11 +132,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -141,23 +154,30 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hypertextový odkaz" xfId="2" builtinId="8"/>
     <cellStyle name="Měna" xfId="1" builtinId="4"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="10">
     <dxf>
-      <numFmt numFmtId="169" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -167,6 +187,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -206,86 +230,6 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -300,16 +244,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabulka1" displayName="Tabulka1" ref="A1:G34" totalsRowShown="0" headerRowDxfId="8" dataDxfId="3">
-  <autoFilter ref="A1:G34"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabulka1" displayName="Tabulka1" ref="A1:H34" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H34"/>
+  <tableColumns count="8">
     <tableColumn id="1" name="Součástka" dataDxfId="7"/>
     <tableColumn id="2" name="Odkaz" dataDxfId="6"/>
-    <tableColumn id="3" name="Počet" dataDxfId="2"/>
-    <tableColumn id="4" name="Cena celkem" dataDxfId="0" dataCellStyle="Měna"/>
-    <tableColumn id="5" name="Objednáno" dataDxfId="1"/>
-    <tableColumn id="6" name="Odesláno" dataDxfId="5"/>
-    <tableColumn id="7" name="Přijato" dataDxfId="4"/>
+    <tableColumn id="3" name="Počet" dataDxfId="5"/>
+    <tableColumn id="4" name="Cena celkem" dataDxfId="4" dataCellStyle="Měna"/>
+    <tableColumn id="5" name="Objednáno" dataDxfId="3"/>
+    <tableColumn id="6" name="Odesláno" dataDxfId="2"/>
+    <tableColumn id="9" name="Předpokládané přijetí" dataDxfId="0">
+      <calculatedColumnFormula>Tabulka1[[#This Row],[Odesláno]]+30</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Přijato" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -581,22 +528,26 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" style="4" customWidth="1"/>
-    <col min="2" max="3" width="21.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11" style="4" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" style="7" customWidth="1"/>
-    <col min="5" max="7" width="21.7109375" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="5" max="5" width="19.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -615,15 +566,18 @@
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1">
@@ -636,13 +590,13 @@
         <v>43066</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1">
@@ -657,13 +611,17 @@
       <c r="F3" s="5">
         <v>43073</v>
       </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="5">
+        <f>Tabulka1[[#This Row],[Odesláno]]+30</f>
+        <v>43103</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1">
@@ -678,13 +636,17 @@
       <c r="F4" s="5">
         <v>43070</v>
       </c>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="5">
+        <f>Tabulka1[[#This Row],[Odesláno]]+30</f>
+        <v>43100</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1">
@@ -699,287 +661,297 @@
       <c r="F5" s="5">
         <v>43069</v>
       </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="5">
+        <f>Tabulka1[[#This Row],[Odesláno]]+30</f>
+        <v>43099</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D48" s="8"/>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="8"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added approximate time of delivery
</commit_message>
<xml_diff>
--- a/Dokumentace/Dokumentační podklady/Objednané součástky/Sledování součástek.xlsx
+++ b/Dokumentace/Dokumentační podklady/Objednané součástky/Sledování součástek.xlsx
@@ -177,10 +177,10 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -253,10 +253,10 @@
     <tableColumn id="4" name="Cena celkem" dataDxfId="4" dataCellStyle="Měna"/>
     <tableColumn id="5" name="Objednáno" dataDxfId="3"/>
     <tableColumn id="6" name="Odesláno" dataDxfId="2"/>
-    <tableColumn id="9" name="Předpokládané přijetí" dataDxfId="0">
+    <tableColumn id="9" name="Předpokládané přijetí" dataDxfId="1">
       <calculatedColumnFormula>Tabulka1[[#This Row],[Odesláno]]+30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Přijato" dataDxfId="1"/>
+    <tableColumn id="7" name="Přijato" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -531,7 +531,7 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated information about my work
</commit_message>
<xml_diff>
--- a/Dokumentace/Dokumentační podklady/Objednané součástky/Sledování součástek.xlsx
+++ b/Dokumentace/Dokumentační podklady/Objednané součástky/Sledování součástek.xlsx
@@ -646,7 +646,9 @@
         <f>Tabulka1[[#This Row],[Odesláno]]+30</f>
         <v>43100</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="5">
+        <v>43091</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">

</xml_diff>

<commit_message>
Updated parts tracking information
</commit_message>
<xml_diff>
--- a/Dokumentace/Dokumentační podklady/Objednané součástky/Sledování součástek.xlsx
+++ b/Dokumentace/Dokumentační podklady/Objednané součástky/Sledování součástek.xlsx
@@ -531,7 +531,7 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +621,9 @@
         <f>Tabulka1[[#This Row],[Odesláno]]+30</f>
         <v>43103</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="H3" s="5">
+        <v>43116</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">

</xml_diff>